<commit_message>
add visualization + sample mini batch size benchmarks
</commit_message>
<xml_diff>
--- a/training/visualization/benchmarks.xlsx
+++ b/training/visualization/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacky\Desktop\results\training\visualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4995A2B-13F9-4C0E-97C3-1322E8041A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ABBA32-7025-4552-B757-A6B1CEE38D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="3750" windowWidth="21600" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t xml:space="preserve">16 actors, collect 100 trajectories, sample 500 trajectories, deque of 5000 </t>
   </si>
@@ -51,6 +51,24 @@
   </si>
   <si>
     <t>Round 500, Training Time: 136.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 actors, collect 100 trajectories, sample 1000 trajectories, deque of 5000 </t>
+  </si>
+  <si>
+    <t>Round 500, Training Time: 148.66</t>
+  </si>
+  <si>
+    <t>Round 500, Training Time: 95.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 actors, collect 100 trajectories, sample 2000 trajectories, deque of 5000 </t>
+  </si>
+  <si>
+    <t>Round 500, Training Time: 95.97</t>
+  </si>
+  <si>
+    <t>Round 500, Training Time: 191.55</t>
   </si>
 </sst>
 </file>
@@ -368,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,9 +420,45 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <f>(136.95-94.22)/136.95</f>
-        <v>0.3120116830960204</v>
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>